<commit_message>
Saving DF with predictions to database
</commit_message>
<xml_diff>
--- a/data/azagorowski_data/df2_industrial_production.xlsx
+++ b/data/azagorowski_data/df2_industrial_production.xlsx
@@ -427,10 +427,10 @@
         <v>92.19389388350932</v>
       </c>
       <c r="E2">
-        <v>91.4427114388368</v>
+        <v>91.5269977855682</v>
       </c>
       <c r="F2">
-        <v>92.89032491297094</v>
+        <v>92.90151707871766</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -447,10 +447,10 @@
         <v>92.39843619557102</v>
       </c>
       <c r="E3">
-        <v>91.7392218790766</v>
+        <v>91.7041257794518</v>
       </c>
       <c r="F3">
-        <v>93.13603959608015</v>
+        <v>93.10484429868022</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -467,10 +467,10 @@
         <v>92.91851022506665</v>
       </c>
       <c r="E4">
-        <v>92.25266216526717</v>
+        <v>92.20397598384967</v>
       </c>
       <c r="F4">
-        <v>93.58468469321804</v>
+        <v>93.65828816872155</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -487,10 +487,10 @@
         <v>93.46723090237175</v>
       </c>
       <c r="E5">
-        <v>92.75363185078989</v>
+        <v>92.80657945415146</v>
       </c>
       <c r="F5">
-        <v>94.10293642054232</v>
+        <v>94.13685606045212</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -507,10 +507,10 @@
         <v>93.90307717910795</v>
       </c>
       <c r="E6">
-        <v>93.25004589283681</v>
+        <v>93.21082580820556</v>
       </c>
       <c r="F6">
-        <v>94.59150916659699</v>
+        <v>94.65934091811582</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -527,10 +527,10 @@
         <v>93.74848014928553</v>
       </c>
       <c r="E7">
-        <v>93.05430697385042</v>
+        <v>93.04753541230866</v>
       </c>
       <c r="F7">
-        <v>94.44950128769297</v>
+        <v>94.466798498071</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -547,10 +547,10 @@
         <v>94.46451537264844</v>
       </c>
       <c r="E8">
-        <v>93.75662388936475</v>
+        <v>93.76764264594105</v>
       </c>
       <c r="F8">
-        <v>95.15177273719868</v>
+        <v>95.15074816542435</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -567,10 +567,10 @@
         <v>94.749907750098</v>
       </c>
       <c r="E9">
-        <v>93.96668424401489</v>
+        <v>94.06519618522708</v>
       </c>
       <c r="F9">
-        <v>95.48908606998049</v>
+        <v>95.49231303519073</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -587,10 +587,10 @@
         <v>94.75650365739834</v>
       </c>
       <c r="E10">
-        <v>94.01094550594392</v>
+        <v>94.06594624759373</v>
       </c>
       <c r="F10">
-        <v>95.4536666707652</v>
+        <v>95.42602126926955</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -607,10 +607,10 @@
         <v>94.94032951030093</v>
       </c>
       <c r="E11">
-        <v>94.24269329518114</v>
+        <v>94.22420205274381</v>
       </c>
       <c r="F11">
-        <v>95.67406807044702</v>
+        <v>95.68100886053546</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -627,10 +627,10 @@
         <v>95.32877037496498</v>
       </c>
       <c r="E12">
-        <v>94.60384994709717</v>
+        <v>94.62879081257505</v>
       </c>
       <c r="F12">
-        <v>95.99772278154646</v>
+        <v>96.05365009959445</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -647,10 +647,10 @@
         <v>95.62635621540672</v>
       </c>
       <c r="E13">
-        <v>94.90328156633355</v>
+        <v>94.96251797875151</v>
       </c>
       <c r="F13">
-        <v>96.27681237771883</v>
+        <v>96.35886782246176</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -667,10 +667,10 @@
         <v>96.07949535757918</v>
       </c>
       <c r="E14">
-        <v>95.34804876621335</v>
+        <v>95.44033664975274</v>
       </c>
       <c r="F14">
-        <v>96.78766664585962</v>
+        <v>96.7589991353946</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -687,10 +687,10 @@
         <v>95.95749238177474</v>
       </c>
       <c r="E15">
-        <v>95.23015210323975</v>
+        <v>95.24267147535589</v>
       </c>
       <c r="F15">
-        <v>96.67368049203144</v>
+        <v>96.67467369438754</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -707,10 +707,10 @@
         <v>96.42727984973716</v>
       </c>
       <c r="E16">
-        <v>95.70295069896555</v>
+        <v>95.73882444415734</v>
       </c>
       <c r="F16">
-        <v>97.09157747974517</v>
+        <v>97.12828663459875</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -727,10 +727,10 @@
         <v>96.44148387220017</v>
       </c>
       <c r="E17">
-        <v>95.78641749799358</v>
+        <v>95.72105790530607</v>
       </c>
       <c r="F17">
-        <v>97.13509186054999</v>
+        <v>97.12137268123031</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -747,10 +747,10 @@
         <v>96.72100774942896</v>
       </c>
       <c r="E18">
-        <v>95.99803172477088</v>
+        <v>95.98541173512936</v>
       </c>
       <c r="F18">
-        <v>97.42385261076153</v>
+        <v>97.45800502129526</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -767,10 +767,10 @@
         <v>96.86308965479202</v>
       </c>
       <c r="E19">
-        <v>96.10093868408748</v>
+        <v>96.13621547497132</v>
       </c>
       <c r="F19">
-        <v>97.57233192546008</v>
+        <v>97.57578248287291</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -787,10 +787,10 @@
         <v>97.33138779792002</v>
       </c>
       <c r="E20">
-        <v>96.57473567607205</v>
+        <v>96.62716214559795</v>
       </c>
       <c r="F20">
-        <v>98.06896281211318</v>
+        <v>98.02060219363699</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -807,10 +807,10 @@
         <v>97.71641427217183</v>
       </c>
       <c r="E21">
-        <v>97.05969249836903</v>
+        <v>97.0331080790086</v>
       </c>
       <c r="F21">
-        <v>98.4044059779513</v>
+        <v>98.43580074208116</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -827,10 +827,10 @@
         <v>98.02218724050148</v>
       </c>
       <c r="E22">
-        <v>97.34093580168586</v>
+        <v>97.32967423670178</v>
       </c>
       <c r="F22">
-        <v>98.73544277696482</v>
+        <v>98.7386848292759</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -847,10 +847,10 @@
         <v>98.23547806589448</v>
       </c>
       <c r="E23">
-        <v>97.56114899874393</v>
+        <v>97.50812270281284</v>
       </c>
       <c r="F23">
-        <v>98.91377460568415</v>
+        <v>98.93571314540122</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -867,10 +867,10 @@
         <v>98.23196344039239</v>
       </c>
       <c r="E24">
-        <v>97.49869644962867</v>
+        <v>97.53832463850435</v>
       </c>
       <c r="F24">
-        <v>98.96622756090071</v>
+        <v>98.90304648137325</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -887,10 +887,10 @@
         <v>98.57340708508417</v>
       </c>
       <c r="E25">
-        <v>97.9202021860258</v>
+        <v>97.86774191955908</v>
       </c>
       <c r="F25">
-        <v>99.29668020288314</v>
+        <v>99.22477456913686</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -907,10 +907,10 @@
         <v>98.68371738809371</v>
       </c>
       <c r="E26">
-        <v>97.96569870393267</v>
+        <v>97.96031738210857</v>
       </c>
       <c r="F26">
-        <v>99.35738947444946</v>
+        <v>99.37378305181686</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -927,10 +927,10 @@
         <v>99.03423767924106</v>
       </c>
       <c r="E27">
-        <v>98.29570797870952</v>
+        <v>98.38058949906598</v>
       </c>
       <c r="F27">
-        <v>99.73873153856158</v>
+        <v>99.71463843274122</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -947,10 +947,10 @@
         <v>99.08526029347375</v>
       </c>
       <c r="E28">
-        <v>98.39946828313718</v>
+        <v>98.3471420199587</v>
       </c>
       <c r="F28">
-        <v>99.76846214889221</v>
+        <v>99.7641459703086</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -967,10 +967,10 @@
         <v>99.6735874512198</v>
       </c>
       <c r="E29">
-        <v>98.96956478988578</v>
+        <v>98.97219423671989</v>
       </c>
       <c r="F29">
-        <v>100.393949506173</v>
+        <v>100.3939234765622</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -987,10 +987,10 @@
         <v>99.66229123574901</v>
       </c>
       <c r="E30">
-        <v>98.98291924419667</v>
+        <v>98.9837239934652</v>
       </c>
       <c r="F30">
-        <v>100.3527428516086</v>
+        <v>100.3389012076552</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1007,10 +1007,10 @@
         <v>99.8196446290702</v>
       </c>
       <c r="E31">
-        <v>99.07132842453238</v>
+        <v>99.09877484386801</v>
       </c>
       <c r="F31">
-        <v>100.4908213242304</v>
+        <v>100.5640299587716</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1027,10 +1027,10 @@
         <v>100.100669654287</v>
       </c>
       <c r="E32">
-        <v>99.46138559636165</v>
+        <v>99.38436160880009</v>
       </c>
       <c r="F32">
-        <v>100.7907020682197</v>
+        <v>100.7803412898898</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1047,10 +1047,10 @@
         <v>99.98470078619887</v>
       </c>
       <c r="E33">
-        <v>99.24579772851988</v>
+        <v>99.24516823047102</v>
       </c>
       <c r="F33">
-        <v>100.6789538849934</v>
+        <v>100.6938963993911</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1067,10 +1067,10 @@
         <v>100.3099638116455</v>
       </c>
       <c r="E34">
-        <v>99.61477825747741</v>
+        <v>99.64136558229931</v>
       </c>
       <c r="F34">
-        <v>101.0154894052442</v>
+        <v>101.0082159101969</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1087,10 +1087,10 @@
         <v>100.395628596271</v>
       </c>
       <c r="E35">
-        <v>99.73234967304417</v>
+        <v>99.69459978979106</v>
       </c>
       <c r="F35">
-        <v>101.0881062079998</v>
+        <v>101.0611084138579</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1107,10 +1107,10 @@
         <v>100.9743169791002</v>
       </c>
       <c r="E36">
-        <v>100.2339845096796</v>
+        <v>100.2634108065455</v>
       </c>
       <c r="F36">
-        <v>101.6691909449063</v>
+        <v>101.7212869849845</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1127,10 +1127,10 @@
         <v>101.6375286954041</v>
       </c>
       <c r="E37">
-        <v>100.9563996550953</v>
+        <v>100.8877359181861</v>
       </c>
       <c r="F37">
-        <v>102.3333615487041</v>
+        <v>102.2971534992837</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1147,10 +1147,10 @@
         <v>100.8731406633935</v>
       </c>
       <c r="E38">
-        <v>100.226676678724</v>
+        <v>100.2007241388901</v>
       </c>
       <c r="F38">
-        <v>101.6086079888026</v>
+        <v>101.5911406020505</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1167,10 +1167,10 @@
         <v>100.8518228786204</v>
       </c>
       <c r="E39">
-        <v>100.1832701365723</v>
+        <v>100.1651729331909</v>
       </c>
       <c r="F39">
-        <v>101.6084305933437</v>
+        <v>101.5411851374941</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1187,10 +1187,10 @@
         <v>101.2274450892098</v>
       </c>
       <c r="E40">
-        <v>100.5310539026784</v>
+        <v>100.4997832235356</v>
       </c>
       <c r="F40">
-        <v>101.9917853026499</v>
+        <v>101.9186853331259</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1207,10 +1207,10 @@
         <v>101.5882103000654</v>
       </c>
       <c r="E41">
-        <v>100.8750129978488</v>
+        <v>100.8695686992106</v>
       </c>
       <c r="F41">
-        <v>102.297125680169</v>
+        <v>102.2879428070896</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1227,10 +1227,10 @@
         <v>101.7768699785079</v>
       </c>
       <c r="E42">
-        <v>101.0496752114804</v>
+        <v>101.0823268116365</v>
       </c>
       <c r="F42">
-        <v>102.455758345027</v>
+        <v>102.4298078974792</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1247,10 +1247,10 @@
         <v>102.3090204432043</v>
       </c>
       <c r="E43">
-        <v>101.5333433227916</v>
+        <v>101.624191044118</v>
       </c>
       <c r="F43">
-        <v>103.0390152505948</v>
+        <v>103.004499757776</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1267,10 +1267,10 @@
         <v>102.0957851467453</v>
       </c>
       <c r="E44">
-        <v>101.3867102513954</v>
+        <v>101.3867190779733</v>
       </c>
       <c r="F44">
-        <v>102.7688171510421</v>
+        <v>102.7299430457491</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1287,10 +1287,10 @@
         <v>102.5310665467924</v>
       </c>
       <c r="E45">
-        <v>101.8320422963405</v>
+        <v>101.8145319986811</v>
       </c>
       <c r="F45">
-        <v>103.2181541613848</v>
+        <v>103.2385862706778</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1307,10 +1307,10 @@
         <v>102.4694178905076</v>
       </c>
       <c r="E46">
-        <v>101.7631166634644</v>
+        <v>101.6957813791726</v>
       </c>
       <c r="F46">
-        <v>103.1566638627535</v>
+        <v>103.1755382357041</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1327,10 +1327,10 @@
         <v>102.7195101900071</v>
       </c>
       <c r="E47">
-        <v>101.9903206037787</v>
+        <v>102.0313684220315</v>
       </c>
       <c r="F47">
-        <v>103.3808130991206</v>
+        <v>103.388796379487</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1347,10 +1347,10 @@
         <v>103.1607653811431</v>
       </c>
       <c r="E48">
-        <v>102.4352446430454</v>
+        <v>102.4636310501822</v>
       </c>
       <c r="F48">
-        <v>103.8923572976033</v>
+        <v>103.8322909536915</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1367,10 +1367,10 @@
         <v>103.6790949768123</v>
       </c>
       <c r="E49">
-        <v>102.9447426380246</v>
+        <v>102.9941634170408</v>
       </c>
       <c r="F49">
-        <v>104.3785057541946</v>
+        <v>104.4220556722415</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1387,10 +1387,10 @@
         <v>103.4910729057184</v>
       </c>
       <c r="E50">
-        <v>102.7660800391495</v>
+        <v>102.7586029305675</v>
       </c>
       <c r="F50">
-        <v>104.1396440556559</v>
+        <v>104.1865522032137</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1407,10 +1407,10 @@
         <v>104.0649964307632</v>
       </c>
       <c r="E51">
-        <v>103.3683429204612</v>
+        <v>103.3077108273885</v>
       </c>
       <c r="F51">
-        <v>104.7917361400613</v>
+        <v>104.7449580783611</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1427,10 +1427,10 @@
         <v>104.5315226753178</v>
       </c>
       <c r="E52">
-        <v>103.7994814774792</v>
+        <v>103.7971226470473</v>
       </c>
       <c r="F52">
-        <v>105.2194487736644</v>
+        <v>105.2096088590155</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1447,10 +1447,10 @@
         <v>104.3172247804642</v>
       </c>
       <c r="E53">
-        <v>103.5742897287198</v>
+        <v>103.6130896800396</v>
       </c>
       <c r="F53">
-        <v>105.0023186664915</v>
+        <v>105.0070650250594</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1467,10 +1467,10 @@
         <v>104.7421973673591</v>
       </c>
       <c r="E54">
-        <v>104.0711581227345</v>
+        <v>104.0303750025691</v>
       </c>
       <c r="F54">
-        <v>105.4578748004494</v>
+        <v>105.463303428025</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1487,10 +1487,10 @@
         <v>104.8912395226288</v>
       </c>
       <c r="E55">
-        <v>104.1785910880748</v>
+        <v>104.2170617867759</v>
       </c>
       <c r="F55">
-        <v>105.5962672149121</v>
+        <v>105.5331373771613</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1507,10 +1507,10 @@
         <v>105.1404765714212</v>
       </c>
       <c r="E56">
-        <v>104.4144113164422</v>
+        <v>104.5047051038136</v>
       </c>
       <c r="F56">
-        <v>105.8062797814209</v>
+        <v>105.8140335011798</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1527,10 +1527,10 @@
         <v>105.4841985339554</v>
       </c>
       <c r="E57">
-        <v>104.739672322309</v>
+        <v>104.8531051683751</v>
       </c>
       <c r="F57">
-        <v>106.1760695189533</v>
+        <v>106.2104506252483</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1547,10 +1547,10 @@
         <v>105.4973675125884</v>
       </c>
       <c r="E58">
-        <v>104.8253667083342</v>
+        <v>104.7613937689442</v>
       </c>
       <c r="F58">
-        <v>106.1708408936031</v>
+        <v>106.1651374443079</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1567,10 +1567,10 @@
         <v>105.7837517503081</v>
       </c>
       <c r="E59">
-        <v>105.0320055736178</v>
+        <v>105.0186328428207</v>
       </c>
       <c r="F59">
-        <v>106.4541364526183</v>
+        <v>106.4762596015115</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1587,10 +1587,10 @@
         <v>106.164264102181</v>
       </c>
       <c r="E60">
-        <v>105.5276663145985</v>
+        <v>105.4618210964351</v>
       </c>
       <c r="F60">
-        <v>106.8660895563965</v>
+        <v>106.8764691975942</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1607,10 +1607,10 @@
         <v>105.5190833962537</v>
       </c>
       <c r="E61">
-        <v>104.7931618608168</v>
+        <v>104.8090999239513</v>
       </c>
       <c r="F61">
-        <v>106.2512268536867</v>
+        <v>106.2189606098823</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -1627,10 +1627,10 @@
         <v>105.3986486509047</v>
       </c>
       <c r="E62">
-        <v>104.6727009250992</v>
+        <v>104.6569263963423</v>
       </c>
       <c r="F62">
-        <v>106.0913312485024</v>
+        <v>106.0405288585954</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -1647,10 +1647,10 @@
         <v>105.2029749474363</v>
       </c>
       <c r="E63">
-        <v>104.4835055308618</v>
+        <v>104.4552060942594</v>
       </c>
       <c r="F63">
-        <v>105.8922440224344</v>
+        <v>105.9081156017997</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -1667,10 +1667,10 @@
         <v>105.2378010168115</v>
       </c>
       <c r="E64">
-        <v>104.5129492123367</v>
+        <v>104.5215508299663</v>
       </c>
       <c r="F64">
-        <v>105.9216131650671</v>
+        <v>105.9517820936497</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -1687,10 +1687,10 @@
         <v>104.6360849132248</v>
       </c>
       <c r="E65">
-        <v>103.8989473407113</v>
+        <v>103.9143529819775</v>
       </c>
       <c r="F65">
-        <v>105.3949956959692</v>
+        <v>105.3313201292689</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -1707,10 +1707,10 @@
         <v>104.2921287358119</v>
       </c>
       <c r="E66">
-        <v>103.5766145089809</v>
+        <v>103.608078787578</v>
       </c>
       <c r="F66">
-        <v>104.9867729228463</v>
+        <v>104.9976156294185</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -1727,10 +1727,10 @@
         <v>104.0185070011808</v>
       </c>
       <c r="E67">
-        <v>103.3132096621322</v>
+        <v>103.2990049477632</v>
       </c>
       <c r="F67">
-        <v>104.7520641684324</v>
+        <v>104.6983372943671</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -1747,10 +1747,10 @@
         <v>104.1123642840596</v>
       </c>
       <c r="E68">
-        <v>103.3758798496804</v>
+        <v>103.4624076756065</v>
       </c>
       <c r="F68">
-        <v>104.8358536665936</v>
+        <v>104.8200070788962</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -1767,10 +1767,10 @@
         <v>104.4444926075182</v>
       </c>
       <c r="E69">
-        <v>103.724193560323</v>
+        <v>103.7628304123353</v>
       </c>
       <c r="F69">
-        <v>105.1568922170911</v>
+        <v>105.2024205679319</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -1787,10 +1787,10 @@
         <v>103.5649676490684</v>
       </c>
       <c r="E70">
-        <v>102.9201152114935</v>
+        <v>102.7988163531733</v>
       </c>
       <c r="F70">
-        <v>104.318550256657</v>
+        <v>104.2286209864895</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -1807,10 +1807,10 @@
         <v>103.3587273899124</v>
       </c>
       <c r="E71">
-        <v>102.6642313467373</v>
+        <v>102.6610954460626</v>
       </c>
       <c r="F71">
-        <v>104.0714107928271</v>
+        <v>104.0781929269822</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -1827,10 +1827,10 @@
         <v>103.2365724566524</v>
       </c>
       <c r="E72">
-        <v>102.5679971770435</v>
+        <v>102.5085116186152</v>
       </c>
       <c r="F72">
-        <v>103.9671536667734</v>
+        <v>103.9434123877294</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -1847,10 +1847,10 @@
         <v>102.7025630953112</v>
       </c>
       <c r="E73">
-        <v>101.9379246809448</v>
+        <v>102.0007360369466</v>
       </c>
       <c r="F73">
-        <v>103.3959641895934</v>
+        <v>103.4068226187001</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -1867,10 +1867,10 @@
         <v>102.4763184349345</v>
       </c>
       <c r="E74">
-        <v>101.7374047607481</v>
+        <v>101.8040085489738</v>
       </c>
       <c r="F74">
-        <v>103.1690361819411</v>
+        <v>103.1475198171244</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -1887,10 +1887,10 @@
         <v>102.4480271767428</v>
       </c>
       <c r="E75">
-        <v>101.7270680484153</v>
+        <v>101.7439151415083</v>
       </c>
       <c r="F75">
-        <v>103.1214946773809</v>
+        <v>103.0704135715237</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -1907,10 +1907,10 @@
         <v>101.8995879615612</v>
       </c>
       <c r="E76">
-        <v>101.1792293953477</v>
+        <v>101.1447121765166</v>
       </c>
       <c r="F76">
-        <v>102.5836930659152</v>
+        <v>102.5972685410186</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -1927,10 +1927,10 @@
         <v>102.1608600837188</v>
       </c>
       <c r="E77">
-        <v>101.4168470245121</v>
+        <v>101.4401986128229</v>
       </c>
       <c r="F77">
-        <v>102.8310767379729</v>
+        <v>102.8445806049583</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -1947,10 +1947,10 @@
         <v>102.0478732511678</v>
       </c>
       <c r="E78">
-        <v>101.3314263299105</v>
+        <v>101.3148096133255</v>
       </c>
       <c r="F78">
-        <v>102.7691645437315</v>
+        <v>102.7163385447086</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -1967,10 +1967,10 @@
         <v>101.8953972443522</v>
       </c>
       <c r="E79">
-        <v>101.1715790499466</v>
+        <v>101.170708532703</v>
       </c>
       <c r="F79">
-        <v>102.578646710137</v>
+        <v>102.5835811646582</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -1987,10 +1987,10 @@
         <v>101.8491590484345</v>
       </c>
       <c r="E80">
-        <v>101.0884435552707</v>
+        <v>101.1599173948699</v>
       </c>
       <c r="F80">
-        <v>102.5801782095608</v>
+        <v>102.5448526952305</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2007,10 +2007,10 @@
         <v>101.6235772860025</v>
       </c>
       <c r="E81">
-        <v>100.9143586763288</v>
+        <v>100.939240825288</v>
       </c>
       <c r="F81">
-        <v>102.3220628829862</v>
+        <v>102.2937329846441</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2027,10 +2027,10 @@
         <v>101.6363875373307</v>
       </c>
       <c r="E82">
-        <v>100.9305662976743</v>
+        <v>100.9307362181115</v>
       </c>
       <c r="F82">
-        <v>102.3678981239234</v>
+        <v>102.343705519973</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -2047,10 +2047,10 @@
         <v>102.3151019151971</v>
       </c>
       <c r="E83">
-        <v>101.6479176082238</v>
+        <v>101.6463877011795</v>
       </c>
       <c r="F83">
-        <v>103.0606119333831</v>
+        <v>103.0354786919097</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2067,10 +2067,10 @@
         <v>102.1237322792421</v>
       </c>
       <c r="E84">
-        <v>101.4088720734258</v>
+        <v>101.4363085979279</v>
       </c>
       <c r="F84">
-        <v>102.8342131995067</v>
+        <v>102.7604239058582</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -2087,10 +2087,10 @@
         <v>102.7692579282935</v>
       </c>
       <c r="E85">
-        <v>102.0729883914375</v>
+        <v>102.1132978923072</v>
       </c>
       <c r="F85">
-        <v>103.4465156028356</v>
+        <v>103.4374590342959</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -2107,10 +2107,10 @@
         <v>102.3014694397327</v>
       </c>
       <c r="E86">
-        <v>101.604704365661</v>
+        <v>101.5522632648815</v>
       </c>
       <c r="F86">
-        <v>102.989071535015</v>
+        <v>103.0265859654067</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -2127,10 +2127,10 @@
         <v>102.2745383237832</v>
       </c>
       <c r="E87">
-        <v>101.5916003159399</v>
+        <v>101.570106369479</v>
       </c>
       <c r="F87">
-        <v>103.0473878376482</v>
+        <v>102.9797524803961</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2147,10 +2147,10 @@
         <v>102.7664439827677</v>
       </c>
       <c r="E88">
-        <v>102.0629710269841</v>
+        <v>102.0793047333723</v>
       </c>
       <c r="F88">
-        <v>103.5466644699999</v>
+        <v>103.5054959173189</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2167,10 +2167,10 @@
         <v>103.6846178319243</v>
       </c>
       <c r="E89">
-        <v>102.994013262175</v>
+        <v>102.9181206056183</v>
       </c>
       <c r="F89">
-        <v>104.395006094008</v>
+        <v>104.3500023338057</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -2187,10 +2187,10 @@
         <v>103.6331510382959</v>
       </c>
       <c r="E90">
-        <v>102.9325610222662</v>
+        <v>102.9277819841413</v>
       </c>
       <c r="F90">
-        <v>104.3291991871332</v>
+        <v>104.3325318401918</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -2207,10 +2207,10 @@
         <v>104.3177890277553</v>
       </c>
       <c r="E91">
-        <v>103.6745803890312</v>
+        <v>103.5775256809891</v>
       </c>
       <c r="F91">
-        <v>104.9713852242324</v>
+        <v>105.0486618525938</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -2227,10 +2227,10 @@
         <v>105.0419173224172</v>
       </c>
       <c r="E92">
-        <v>104.3377175492593</v>
+        <v>104.3065611542166</v>
       </c>
       <c r="F92">
-        <v>105.7460433982199</v>
+        <v>105.7466769333659</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -2247,10 +2247,10 @@
         <v>104.9944924828975</v>
       </c>
       <c r="E93">
-        <v>104.2877309187604</v>
+        <v>104.3103127598464</v>
       </c>
       <c r="F93">
-        <v>105.7114702670492</v>
+        <v>105.6736750084613</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -2267,10 +2267,10 @@
         <v>105.2714962129347</v>
       </c>
       <c r="E94">
-        <v>104.5566604944701</v>
+        <v>104.6335701616995</v>
       </c>
       <c r="F94">
-        <v>106.0046105193608</v>
+        <v>105.9963120241285</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -2287,10 +2287,10 @@
         <v>106.0272991559107</v>
       </c>
       <c r="E95">
-        <v>105.3488732550551</v>
+        <v>105.3086912898524</v>
       </c>
       <c r="F95">
-        <v>106.7928798020031</v>
+        <v>106.6830730811679</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -2307,10 +2307,10 @@
         <v>106.555233731514</v>
       </c>
       <c r="E96">
-        <v>105.8615910176153</v>
+        <v>105.8910705728811</v>
       </c>
       <c r="F96">
-        <v>107.2174217820633</v>
+        <v>107.2521457153791</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -2327,10 +2327,10 @@
         <v>107.1219377798666</v>
       </c>
       <c r="E97">
-        <v>106.36184499267</v>
+        <v>106.459100483577</v>
       </c>
       <c r="F97">
-        <v>107.8263722549444</v>
+        <v>107.8304067589977</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -2347,10 +2347,10 @@
         <v>106.8871573567382</v>
       </c>
       <c r="E98">
-        <v>106.2092306399132</v>
+        <v>106.2077025634197</v>
       </c>
       <c r="F98">
-        <v>107.6227304109391</v>
+        <v>107.6147051932386</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -2367,10 +2367,10 @@
         <v>107.2114826499776</v>
       </c>
       <c r="E99">
-        <v>106.4990136292565</v>
+        <v>106.5071309727215</v>
       </c>
       <c r="F99">
-        <v>107.8993818549716</v>
+        <v>107.9460132974194</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -2387,10 +2387,10 @@
         <v>107.5762883995121</v>
       </c>
       <c r="E100">
-        <v>106.9097104228551</v>
+        <v>106.8434672211346</v>
       </c>
       <c r="F100">
-        <v>108.2728623347466</v>
+        <v>108.2295837012832</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -2407,10 +2407,10 @@
         <v>107.6122954328949</v>
       </c>
       <c r="E101">
-        <v>106.8993626409421</v>
+        <v>106.8783400168468</v>
       </c>
       <c r="F101">
-        <v>108.2714741507786</v>
+        <v>108.3268290660903</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -2427,10 +2427,10 @@
         <v>107.5188587905234</v>
       </c>
       <c r="E102">
-        <v>106.7712555269815</v>
+        <v>106.805705489604</v>
       </c>
       <c r="F102">
-        <v>108.2019048286392</v>
+        <v>108.2578915178192</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -2447,10 +2447,10 @@
         <v>107.6728991076946</v>
       </c>
       <c r="E103">
-        <v>106.9504194553007</v>
+        <v>106.9919632338275</v>
       </c>
       <c r="F103">
-        <v>108.4539516281123</v>
+        <v>108.393724980945</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -2467,10 +2467,10 @@
         <v>108.104958357304</v>
       </c>
       <c r="E104">
-        <v>107.4157945510448</v>
+        <v>107.4171041066081</v>
       </c>
       <c r="F104">
-        <v>108.7895126007469</v>
+        <v>108.8353350377148</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -2487,10 +2487,10 @@
         <v>108.2017083135553</v>
       </c>
       <c r="E105">
-        <v>107.4988522264538</v>
+        <v>107.5630717411407</v>
       </c>
       <c r="F105">
-        <v>108.9057235025727</v>
+        <v>108.8916252867404</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -2507,10 +2507,10 @@
         <v>108.5309272667882</v>
       </c>
       <c r="E106">
-        <v>107.8185207972401</v>
+        <v>107.8688138889522</v>
       </c>
       <c r="F106">
-        <v>109.2000094789965</v>
+        <v>109.2084467946931</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -2527,10 +2527,10 @@
         <v>108.1880725265816</v>
       </c>
       <c r="E107">
-        <v>107.533328702766</v>
+        <v>107.4826949568138</v>
       </c>
       <c r="F107">
-        <v>108.9105149625755</v>
+        <v>108.9301803811454</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -2547,10 +2547,10 @@
         <v>108.766919062403</v>
       </c>
       <c r="E108">
-        <v>108.0571247492319</v>
+        <v>108.0522937288157</v>
       </c>
       <c r="F108">
-        <v>109.4616364207617</v>
+        <v>109.4982939557343</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -2567,10 +2567,10 @@
         <v>109.1034696822857</v>
       </c>
       <c r="E109">
-        <v>108.4020612117341</v>
+        <v>108.3859190160971</v>
       </c>
       <c r="F109">
-        <v>109.7966347622607</v>
+        <v>109.844239118617</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -2587,10 +2587,10 @@
         <v>108.6146147084751</v>
       </c>
       <c r="E110">
-        <v>107.9279804932169</v>
+        <v>107.8658143794981</v>
       </c>
       <c r="F110">
-        <v>109.3325216094813</v>
+        <v>109.3370143956779</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -2607,10 +2607,10 @@
         <v>108.8718715824796</v>
       </c>
       <c r="E111">
-        <v>108.1417971169617</v>
+        <v>108.1122215681474</v>
       </c>
       <c r="F111">
-        <v>109.5331717384599</v>
+        <v>109.5900282194388</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -2627,10 +2627,10 @@
         <v>109.2501790046248</v>
       </c>
       <c r="E112">
-        <v>108.5537887211248</v>
+        <v>108.5790757351449</v>
       </c>
       <c r="F112">
-        <v>109.9636408933288</v>
+        <v>109.9767693583087</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -2647,10 +2647,10 @@
         <v>109.0946065949522</v>
       </c>
       <c r="E113">
-        <v>108.3799008920826</v>
+        <v>108.3778138960137</v>
       </c>
       <c r="F113">
-        <v>109.8154423004155</v>
+        <v>109.7689509946741</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -2667,10 +2667,10 @@
         <v>109.2102553677619</v>
       </c>
       <c r="E114">
-        <v>108.5175589077248</v>
+        <v>108.4948077287535</v>
       </c>
       <c r="F114">
-        <v>109.9095713835374</v>
+        <v>109.9449015267268</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -2687,10 +2687,10 @@
         <v>109.7455828198247</v>
       </c>
       <c r="E115">
-        <v>109.0808336104459</v>
+        <v>109.050694886483</v>
       </c>
       <c r="F115">
-        <v>110.4370213214546</v>
+        <v>110.4147489802821</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -2707,10 +2707,10 @@
         <v>109.6872003657527</v>
       </c>
       <c r="E116">
-        <v>109.0161075080355</v>
+        <v>108.9796624486792</v>
       </c>
       <c r="F116">
-        <v>110.4190010368139</v>
+        <v>110.3815597735493</v>
       </c>
     </row>
     <row r="117" spans="1:6">
@@ -2727,10 +2727,10 @@
         <v>110.2626325069358</v>
       </c>
       <c r="E117">
-        <v>109.5526234764105</v>
+        <v>109.6195403725468</v>
       </c>
       <c r="F117">
-        <v>110.9567883659657</v>
+        <v>111.0006070441363</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -2747,10 +2747,10 @@
         <v>110.1263145260697</v>
       </c>
       <c r="E118">
-        <v>109.4593360122043</v>
+        <v>109.4482580966732</v>
       </c>
       <c r="F118">
-        <v>110.837780249065</v>
+        <v>110.763582011861</v>
       </c>
     </row>
     <row r="119" spans="1:6">
@@ -2767,10 +2767,10 @@
         <v>109.8786669756402</v>
       </c>
       <c r="E119">
-        <v>109.1322808806835</v>
+        <v>109.2317703163682</v>
       </c>
       <c r="F119">
-        <v>110.5450783592458</v>
+        <v>110.6169888760736</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -2787,10 +2787,10 @@
         <v>110.2544122068744</v>
       </c>
       <c r="E120">
-        <v>109.5655295960993</v>
+        <v>109.5580650658305</v>
       </c>
       <c r="F120">
-        <v>110.9871411802405</v>
+        <v>110.9552066971811</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -2807,10 +2807,10 @@
         <v>110.3802242420797</v>
       </c>
       <c r="E121">
-        <v>109.7027852492912</v>
+        <v>109.6825971610029</v>
       </c>
       <c r="F121">
-        <v>111.1079669863584</v>
+        <v>111.090527395726</v>
       </c>
     </row>
     <row r="122" spans="1:6">
@@ -2827,10 +2827,10 @@
         <v>110.3999067443418</v>
       </c>
       <c r="E122">
-        <v>109.6898194097279</v>
+        <v>109.7197399767551</v>
       </c>
       <c r="F122">
-        <v>111.1186781996093</v>
+        <v>111.0817376894651</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -2844,10 +2844,10 @@
         <v>111.3279300677196</v>
       </c>
       <c r="E123">
-        <v>110.6556760833462</v>
+        <v>110.6019465765201</v>
       </c>
       <c r="F123">
-        <v>112.0378912927993</v>
+        <v>112.0418225759735</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -2861,10 +2861,10 @@
         <v>111.5548372711512</v>
       </c>
       <c r="E124">
-        <v>110.8468248509801</v>
+        <v>110.8765658587355</v>
       </c>
       <c r="F124">
-        <v>112.2824085684653</v>
+        <v>112.2783207766092</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -2878,10 +2878,10 @@
         <v>110.7459079046332</v>
       </c>
       <c r="E125">
-        <v>110.0321904364797</v>
+        <v>109.9962343424272</v>
       </c>
       <c r="F125">
-        <v>111.4428107323867</v>
+        <v>111.4950173946675</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -2895,10 +2895,10 @@
         <v>111.0328904849513</v>
       </c>
       <c r="E126">
-        <v>110.2657677339269</v>
+        <v>110.2719001480418</v>
       </c>
       <c r="F126">
-        <v>111.7900303956201</v>
+        <v>111.7903297563486</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -2912,10 +2912,10 @@
         <v>111.1147227369815</v>
       </c>
       <c r="E127">
-        <v>110.3414884535444</v>
+        <v>110.3248711544056</v>
       </c>
       <c r="F127">
-        <v>111.8571755481908</v>
+        <v>111.9152794299338</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -2929,10 +2929,10 @@
         <v>111.4479696700109</v>
       </c>
       <c r="E128">
-        <v>110.6974613382003</v>
+        <v>110.6394661869638</v>
       </c>
       <c r="F128">
-        <v>112.3242037531178</v>
+        <v>112.2726451992771</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -2946,10 +2946,10 @@
         <v>111.9190226081632</v>
       </c>
       <c r="E129">
-        <v>111.046641597787</v>
+        <v>110.9948356725616</v>
       </c>
       <c r="F129">
-        <v>112.7617402678679</v>
+        <v>112.8056420817375</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -2963,10 +2963,10 @@
         <v>111.838983935599</v>
       </c>
       <c r="E130">
-        <v>110.8656446989494</v>
+        <v>110.9428892875249</v>
       </c>
       <c r="F130">
-        <v>112.7433355728044</v>
+        <v>112.7502291717285</v>
       </c>
     </row>
     <row r="131" spans="1:6">
@@ -2980,10 +2980,10 @@
         <v>111.617052131952</v>
       </c>
       <c r="E131">
-        <v>110.6551672797861</v>
+        <v>110.6414987797315</v>
       </c>
       <c r="F131">
-        <v>112.6443055746098</v>
+        <v>112.6521035203966</v>
       </c>
     </row>
     <row r="132" spans="1:6">
@@ -2997,10 +2997,10 @@
         <v>112.37455272019</v>
       </c>
       <c r="E132">
-        <v>111.3050641250056</v>
+        <v>111.3496300899289</v>
       </c>
       <c r="F132">
-        <v>113.4833190412007</v>
+        <v>113.5627301873892</v>
       </c>
     </row>
     <row r="133" spans="1:6">
@@ -3014,10 +3014,10 @@
         <v>111.7790363004907</v>
       </c>
       <c r="E133">
-        <v>110.54886349857</v>
+        <v>110.7300999207734</v>
       </c>
       <c r="F133">
-        <v>113.0624349700462</v>
+        <v>113.1144752286714</v>
       </c>
     </row>
     <row r="134" spans="1:6">
@@ -3031,10 +3031,10 @@
         <v>112.322790524022</v>
       </c>
       <c r="E134">
-        <v>111.0194743969974</v>
+        <v>111.0827241585224</v>
       </c>
       <c r="F134">
-        <v>113.6320835242253</v>
+        <v>113.6934596816023</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add industrial_prod to db
</commit_message>
<xml_diff>
--- a/data/azagorowski_data/df2_industrial_production.xlsx
+++ b/data/azagorowski_data/df2_industrial_production.xlsx
@@ -427,10 +427,10 @@
         <v>92.19389388350932</v>
       </c>
       <c r="E2">
-        <v>91.5269977855682</v>
+        <v>91.48933140855368</v>
       </c>
       <c r="F2">
-        <v>92.90151707871766</v>
+        <v>92.91444772161584</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -447,10 +447,10 @@
         <v>92.39843619557102</v>
       </c>
       <c r="E3">
-        <v>91.7041257794518</v>
+        <v>91.6762739977716</v>
       </c>
       <c r="F3">
-        <v>93.10484429868022</v>
+        <v>93.0929482477172</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -467,10 +467,10 @@
         <v>92.91851022506665</v>
       </c>
       <c r="E4">
-        <v>92.20397598384967</v>
+        <v>92.21823891373009</v>
       </c>
       <c r="F4">
-        <v>93.65828816872155</v>
+        <v>93.59423770196769</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -487,10 +487,10 @@
         <v>93.46723090237175</v>
       </c>
       <c r="E5">
-        <v>92.80657945415146</v>
+        <v>92.79237794379173</v>
       </c>
       <c r="F5">
-        <v>94.13685606045212</v>
+        <v>94.18029011660145</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -507,10 +507,10 @@
         <v>93.90307717910795</v>
       </c>
       <c r="E6">
-        <v>93.21082580820556</v>
+        <v>93.24334334814968</v>
       </c>
       <c r="F6">
-        <v>94.65934091811582</v>
+        <v>94.59661925369267</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -527,10 +527,10 @@
         <v>93.74848014928553</v>
       </c>
       <c r="E7">
-        <v>93.04753541230866</v>
+        <v>93.04038228067114</v>
       </c>
       <c r="F7">
-        <v>94.466798498071</v>
+        <v>94.46562282683756</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -547,10 +547,10 @@
         <v>94.46451537264844</v>
       </c>
       <c r="E8">
-        <v>93.76764264594105</v>
+        <v>93.78028022973761</v>
       </c>
       <c r="F8">
-        <v>95.15074816542435</v>
+        <v>95.10720355327049</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -567,10 +567,10 @@
         <v>94.749907750098</v>
       </c>
       <c r="E9">
-        <v>94.06519618522708</v>
+        <v>94.07450619788142</v>
       </c>
       <c r="F9">
-        <v>95.49231303519073</v>
+        <v>95.37881180666017</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -587,10 +587,10 @@
         <v>94.75650365739834</v>
       </c>
       <c r="E10">
-        <v>94.06594624759373</v>
+        <v>94.06497342934561</v>
       </c>
       <c r="F10">
-        <v>95.42602126926955</v>
+        <v>95.44132425350807</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -607,10 +607,10 @@
         <v>94.94032951030093</v>
       </c>
       <c r="E11">
-        <v>94.22420205274381</v>
+        <v>94.24478122578299</v>
       </c>
       <c r="F11">
-        <v>95.68100886053546</v>
+        <v>95.63857090979539</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -627,10 +627,10 @@
         <v>95.32877037496498</v>
       </c>
       <c r="E12">
-        <v>94.62879081257505</v>
+        <v>94.59747111506908</v>
       </c>
       <c r="F12">
-        <v>96.05365009959445</v>
+        <v>96.03760471808506</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -647,10 +647,10 @@
         <v>95.62635621540672</v>
       </c>
       <c r="E13">
-        <v>94.96251797875151</v>
+        <v>94.95233810307835</v>
       </c>
       <c r="F13">
-        <v>96.35886782246176</v>
+        <v>96.35204850193999</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -667,10 +667,10 @@
         <v>96.07949535757918</v>
       </c>
       <c r="E14">
-        <v>95.44033664975274</v>
+        <v>95.36657447204951</v>
       </c>
       <c r="F14">
-        <v>96.7589991353946</v>
+        <v>96.78123322817744</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -687,10 +687,10 @@
         <v>95.95749238177474</v>
       </c>
       <c r="E15">
-        <v>95.24267147535589</v>
+        <v>95.27117505772449</v>
       </c>
       <c r="F15">
-        <v>96.67467369438754</v>
+        <v>96.71217636534139</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -707,10 +707,10 @@
         <v>96.42727984973716</v>
       </c>
       <c r="E16">
-        <v>95.73882444415734</v>
+        <v>95.7330825861043</v>
       </c>
       <c r="F16">
-        <v>97.12828663459875</v>
+        <v>97.14524578504043</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -727,10 +727,10 @@
         <v>96.44148387220017</v>
       </c>
       <c r="E17">
-        <v>95.72105790530607</v>
+        <v>95.70311289713963</v>
       </c>
       <c r="F17">
-        <v>97.12137268123031</v>
+        <v>97.13845475161449</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -747,10 +747,10 @@
         <v>96.72100774942896</v>
       </c>
       <c r="E18">
-        <v>95.98541173512936</v>
+        <v>95.97597362509909</v>
       </c>
       <c r="F18">
-        <v>97.45800502129526</v>
+        <v>97.38364137492579</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -767,10 +767,10 @@
         <v>96.86308965479202</v>
       </c>
       <c r="E19">
-        <v>96.13621547497132</v>
+        <v>96.1258333038157</v>
       </c>
       <c r="F19">
-        <v>97.57578248287291</v>
+        <v>97.47523482153326</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -787,10 +787,10 @@
         <v>97.33138779792002</v>
       </c>
       <c r="E20">
-        <v>96.62716214559795</v>
+        <v>96.6612880039317</v>
       </c>
       <c r="F20">
-        <v>98.02060219363699</v>
+        <v>98.00711018301438</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -807,10 +807,10 @@
         <v>97.71641427217183</v>
       </c>
       <c r="E21">
-        <v>97.0331080790086</v>
+        <v>97.02048284854484</v>
       </c>
       <c r="F21">
-        <v>98.43580074208116</v>
+        <v>98.39155771657691</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -827,10 +827,10 @@
         <v>98.02218724050148</v>
       </c>
       <c r="E22">
-        <v>97.32967423670178</v>
+        <v>97.41613004268949</v>
       </c>
       <c r="F22">
-        <v>98.7386848292759</v>
+        <v>98.73981521615013</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -847,10 +847,10 @@
         <v>98.23547806589448</v>
       </c>
       <c r="E23">
-        <v>97.50812270281284</v>
+        <v>97.46457661463364</v>
       </c>
       <c r="F23">
-        <v>98.93571314540122</v>
+        <v>98.8824146836443</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -867,10 +867,10 @@
         <v>98.23196344039239</v>
       </c>
       <c r="E24">
-        <v>97.53832463850435</v>
+        <v>97.5771911370548</v>
       </c>
       <c r="F24">
-        <v>98.90304648137325</v>
+        <v>98.96632622778534</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -887,10 +887,10 @@
         <v>98.57340708508417</v>
       </c>
       <c r="E25">
-        <v>97.86774191955908</v>
+        <v>97.89457544130956</v>
       </c>
       <c r="F25">
-        <v>99.22477456913686</v>
+        <v>99.31878767145594</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -907,10 +907,10 @@
         <v>98.68371738809371</v>
       </c>
       <c r="E26">
-        <v>97.96031738210857</v>
+        <v>98.00209882765482</v>
       </c>
       <c r="F26">
-        <v>99.37378305181686</v>
+        <v>99.37417318320868</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -927,10 +927,10 @@
         <v>99.03423767924106</v>
       </c>
       <c r="E27">
-        <v>98.38058949906598</v>
+        <v>98.3355737237072</v>
       </c>
       <c r="F27">
-        <v>99.71463843274122</v>
+        <v>99.78464754942809</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -947,10 +947,10 @@
         <v>99.08526029347375</v>
       </c>
       <c r="E28">
-        <v>98.3471420199587</v>
+        <v>98.39727441541145</v>
       </c>
       <c r="F28">
-        <v>99.7641459703086</v>
+        <v>99.75921964094462</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -967,10 +967,10 @@
         <v>99.6735874512198</v>
       </c>
       <c r="E29">
-        <v>98.97219423671989</v>
+        <v>99.00234624628602</v>
       </c>
       <c r="F29">
-        <v>100.3939234765622</v>
+        <v>100.3906422617128</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -987,10 +987,10 @@
         <v>99.66229123574901</v>
       </c>
       <c r="E30">
-        <v>98.9837239934652</v>
+        <v>98.94503615797164</v>
       </c>
       <c r="F30">
-        <v>100.3389012076552</v>
+        <v>100.3497025175066</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1007,10 +1007,10 @@
         <v>99.8196446290702</v>
       </c>
       <c r="E31">
-        <v>99.09877484386801</v>
+        <v>99.10483243675446</v>
       </c>
       <c r="F31">
-        <v>100.5640299587716</v>
+        <v>100.5300622221215</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1027,10 +1027,10 @@
         <v>100.100669654287</v>
       </c>
       <c r="E32">
-        <v>99.38436160880009</v>
+        <v>99.3994132421485</v>
       </c>
       <c r="F32">
-        <v>100.7803412898898</v>
+        <v>100.7515296071184</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1047,10 +1047,10 @@
         <v>99.98470078619887</v>
       </c>
       <c r="E33">
-        <v>99.24516823047102</v>
+        <v>99.30482233365736</v>
       </c>
       <c r="F33">
-        <v>100.6938963993911</v>
+        <v>100.7138693215012</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1067,10 +1067,10 @@
         <v>100.3099638116455</v>
       </c>
       <c r="E34">
-        <v>99.64136558229931</v>
+        <v>99.6104378890052</v>
       </c>
       <c r="F34">
-        <v>101.0082159101969</v>
+        <v>100.9714434871674</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1087,10 +1087,10 @@
         <v>100.395628596271</v>
       </c>
       <c r="E35">
-        <v>99.69459978979106</v>
+        <v>99.68663609967886</v>
       </c>
       <c r="F35">
-        <v>101.0611084138579</v>
+        <v>101.1311579568847</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1107,10 +1107,10 @@
         <v>100.9743169791002</v>
       </c>
       <c r="E36">
-        <v>100.2634108065455</v>
+        <v>100.2321092784905</v>
       </c>
       <c r="F36">
-        <v>101.7212869849845</v>
+        <v>101.6740470861317</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1127,10 +1127,10 @@
         <v>101.6375286954041</v>
       </c>
       <c r="E37">
-        <v>100.8877359181861</v>
+        <v>100.9178311071983</v>
       </c>
       <c r="F37">
-        <v>102.2971534992837</v>
+        <v>102.4090525792099</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1147,10 +1147,10 @@
         <v>100.8731406633935</v>
       </c>
       <c r="E38">
-        <v>100.2007241388901</v>
+        <v>100.1499122146231</v>
       </c>
       <c r="F38">
-        <v>101.5911406020505</v>
+        <v>101.5707575025837</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1167,10 +1167,10 @@
         <v>100.8518228786204</v>
       </c>
       <c r="E39">
-        <v>100.1651729331909</v>
+        <v>100.1993235775479</v>
       </c>
       <c r="F39">
-        <v>101.5411851374941</v>
+        <v>101.5863600557257</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1187,10 +1187,10 @@
         <v>101.2274450892098</v>
       </c>
       <c r="E40">
-        <v>100.4997832235356</v>
+        <v>100.5530569164283</v>
       </c>
       <c r="F40">
-        <v>101.9186853331259</v>
+        <v>101.9878305056511</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1207,10 +1207,10 @@
         <v>101.5882103000654</v>
       </c>
       <c r="E41">
-        <v>100.8695686992106</v>
+        <v>100.9034239339483</v>
       </c>
       <c r="F41">
-        <v>102.2879428070896</v>
+        <v>102.2673879431816</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1227,10 +1227,10 @@
         <v>101.7768699785079</v>
       </c>
       <c r="E42">
-        <v>101.0823268116365</v>
+        <v>101.0349703783224</v>
       </c>
       <c r="F42">
-        <v>102.4298078974792</v>
+        <v>102.4839761660165</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1247,10 +1247,10 @@
         <v>102.3090204432043</v>
       </c>
       <c r="E43">
-        <v>101.624191044118</v>
+        <v>101.5620662126771</v>
       </c>
       <c r="F43">
-        <v>103.004499757776</v>
+        <v>103.0229940198695</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1267,10 +1267,10 @@
         <v>102.0957851467453</v>
       </c>
       <c r="E44">
-        <v>101.3867190779733</v>
+        <v>101.3720232419294</v>
       </c>
       <c r="F44">
-        <v>102.7299430457491</v>
+        <v>102.8166176896568</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1287,10 +1287,10 @@
         <v>102.5310665467924</v>
       </c>
       <c r="E45">
-        <v>101.8145319986811</v>
+        <v>101.8249997433435</v>
       </c>
       <c r="F45">
-        <v>103.2385862706778</v>
+        <v>103.2402647295746</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1307,10 +1307,10 @@
         <v>102.4694178905076</v>
       </c>
       <c r="E46">
-        <v>101.6957813791726</v>
+        <v>101.7955172578134</v>
       </c>
       <c r="F46">
-        <v>103.1755382357041</v>
+        <v>103.2139122388769</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1327,10 +1327,10 @@
         <v>102.7195101900071</v>
       </c>
       <c r="E47">
-        <v>102.0313684220315</v>
+        <v>102.0135319674484</v>
       </c>
       <c r="F47">
-        <v>103.388796379487</v>
+        <v>103.4404621949672</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1347,10 +1347,10 @@
         <v>103.1607653811431</v>
       </c>
       <c r="E48">
-        <v>102.4636310501822</v>
+        <v>102.4549139921377</v>
       </c>
       <c r="F48">
-        <v>103.8322909536915</v>
+        <v>103.839360936753</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1367,10 +1367,10 @@
         <v>103.6790949768123</v>
       </c>
       <c r="E49">
-        <v>102.9941634170408</v>
+        <v>102.9877886488125</v>
       </c>
       <c r="F49">
-        <v>104.4220556722415</v>
+        <v>104.3762439048083</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1387,10 +1387,10 @@
         <v>103.4910729057184</v>
       </c>
       <c r="E50">
-        <v>102.7586029305675</v>
+        <v>102.7687811788976</v>
       </c>
       <c r="F50">
-        <v>104.1865522032137</v>
+        <v>104.1996660769876</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1407,10 +1407,10 @@
         <v>104.0649964307632</v>
       </c>
       <c r="E51">
-        <v>103.3077108273885</v>
+        <v>103.3587725334912</v>
       </c>
       <c r="F51">
-        <v>104.7449580783611</v>
+        <v>104.7145197073188</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1427,10 +1427,10 @@
         <v>104.5315226753178</v>
       </c>
       <c r="E52">
-        <v>103.7971226470473</v>
+        <v>103.9240590007589</v>
       </c>
       <c r="F52">
-        <v>105.2096088590155</v>
+        <v>105.2025605315014</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1447,10 +1447,10 @@
         <v>104.3172247804642</v>
       </c>
       <c r="E53">
-        <v>103.6130896800396</v>
+        <v>103.6018069166118</v>
       </c>
       <c r="F53">
-        <v>105.0070650250594</v>
+        <v>105.0568758725337</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1467,10 +1467,10 @@
         <v>104.7421973673591</v>
       </c>
       <c r="E54">
-        <v>104.0303750025691</v>
+        <v>104.048391890355</v>
       </c>
       <c r="F54">
-        <v>105.463303428025</v>
+        <v>105.4269546557435</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1487,10 +1487,10 @@
         <v>104.8912395226288</v>
       </c>
       <c r="E55">
-        <v>104.2170617867759</v>
+        <v>104.1791115481038</v>
       </c>
       <c r="F55">
-        <v>105.5331373771613</v>
+        <v>105.6097059236105</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1507,10 +1507,10 @@
         <v>105.1404765714212</v>
       </c>
       <c r="E56">
-        <v>104.5047051038136</v>
+        <v>104.4553746124191</v>
       </c>
       <c r="F56">
-        <v>105.8140335011798</v>
+        <v>105.8678417399829</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1527,10 +1527,10 @@
         <v>105.4841985339554</v>
       </c>
       <c r="E57">
-        <v>104.8531051683751</v>
+        <v>104.7885378413553</v>
       </c>
       <c r="F57">
-        <v>106.2104506252483</v>
+        <v>106.194530123075</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1547,10 +1547,10 @@
         <v>105.4973675125884</v>
       </c>
       <c r="E58">
-        <v>104.7613937689442</v>
+        <v>104.8615616420633</v>
       </c>
       <c r="F58">
-        <v>106.1651374443079</v>
+        <v>106.1927709905069</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1567,10 +1567,10 @@
         <v>105.7837517503081</v>
       </c>
       <c r="E59">
-        <v>105.0186328428207</v>
+        <v>105.0860179703211</v>
       </c>
       <c r="F59">
-        <v>106.4762596015115</v>
+        <v>106.4622775710191</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1587,10 +1587,10 @@
         <v>106.164264102181</v>
       </c>
       <c r="E60">
-        <v>105.4618210964351</v>
+        <v>105.3873790196008</v>
       </c>
       <c r="F60">
-        <v>106.8764691975942</v>
+        <v>106.8155321390619</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1607,10 +1607,10 @@
         <v>105.5190833962537</v>
       </c>
       <c r="E61">
-        <v>104.8090999239513</v>
+        <v>104.7958263937065</v>
       </c>
       <c r="F61">
-        <v>106.2189606098823</v>
+        <v>106.2383828586357</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -1627,10 +1627,10 @@
         <v>105.3986486509047</v>
       </c>
       <c r="E62">
-        <v>104.6569263963423</v>
+        <v>104.7289377111638</v>
       </c>
       <c r="F62">
-        <v>106.0405288585954</v>
+        <v>106.0789344662861</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -1647,10 +1647,10 @@
         <v>105.2029749474363</v>
       </c>
       <c r="E63">
-        <v>104.4552060942594</v>
+        <v>104.504910449329</v>
       </c>
       <c r="F63">
-        <v>105.9081156017997</v>
+        <v>105.9129395318057</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -1667,10 +1667,10 @@
         <v>105.2378010168115</v>
       </c>
       <c r="E64">
-        <v>104.5215508299663</v>
+        <v>104.5523171160657</v>
       </c>
       <c r="F64">
-        <v>105.9517820936497</v>
+        <v>105.9231088241947</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -1687,10 +1687,10 @@
         <v>104.6360849132248</v>
       </c>
       <c r="E65">
-        <v>103.9143529819775</v>
+        <v>104.0024741850922</v>
       </c>
       <c r="F65">
-        <v>105.3313201292689</v>
+        <v>105.3397178479294</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -1707,10 +1707,10 @@
         <v>104.2921287358119</v>
       </c>
       <c r="E66">
-        <v>103.608078787578</v>
+        <v>103.5795489885018</v>
       </c>
       <c r="F66">
-        <v>104.9976156294185</v>
+        <v>104.9761223744401</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -1727,10 +1727,10 @@
         <v>104.0185070011808</v>
       </c>
       <c r="E67">
-        <v>103.2990049477632</v>
+        <v>103.307897287032</v>
       </c>
       <c r="F67">
-        <v>104.6983372943671</v>
+        <v>104.7127379910111</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -1747,10 +1747,10 @@
         <v>104.1123642840596</v>
       </c>
       <c r="E68">
-        <v>103.4624076756065</v>
+        <v>103.4057373788984</v>
       </c>
       <c r="F68">
-        <v>104.8200070788962</v>
+        <v>104.7706556869455</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -1767,10 +1767,10 @@
         <v>104.4444926075182</v>
       </c>
       <c r="E69">
-        <v>103.7628304123353</v>
+        <v>103.7594342826677</v>
       </c>
       <c r="F69">
-        <v>105.2024205679319</v>
+        <v>105.2239275803411</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -1787,10 +1787,10 @@
         <v>103.5649676490684</v>
       </c>
       <c r="E70">
-        <v>102.7988163531733</v>
+        <v>102.8770436453506</v>
       </c>
       <c r="F70">
-        <v>104.2286209864895</v>
+        <v>104.3043124621678</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -1807,10 +1807,10 @@
         <v>103.3587273899124</v>
       </c>
       <c r="E71">
-        <v>102.6610954460626</v>
+        <v>102.7107567415891</v>
       </c>
       <c r="F71">
-        <v>104.0781929269822</v>
+        <v>103.9862923543372</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -1827,10 +1827,10 @@
         <v>103.2365724566524</v>
       </c>
       <c r="E72">
-        <v>102.5085116186152</v>
+        <v>102.5108263576605</v>
       </c>
       <c r="F72">
-        <v>103.9434123877294</v>
+        <v>103.9104020863809</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -1847,10 +1847,10 @@
         <v>102.7025630953112</v>
       </c>
       <c r="E73">
-        <v>102.0007360369466</v>
+        <v>102.0025433738329</v>
       </c>
       <c r="F73">
-        <v>103.4068226187001</v>
+        <v>103.3648384150725</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -1867,10 +1867,10 @@
         <v>102.4763184349345</v>
       </c>
       <c r="E74">
-        <v>101.8040085489738</v>
+        <v>101.7322586135023</v>
       </c>
       <c r="F74">
-        <v>103.1475198171244</v>
+        <v>103.1848256784123</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -1887,10 +1887,10 @@
         <v>102.4480271767428</v>
       </c>
       <c r="E75">
-        <v>101.7439151415083</v>
+        <v>101.7326951153784</v>
       </c>
       <c r="F75">
-        <v>103.0704135715237</v>
+        <v>103.1405623228393</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -1907,10 +1907,10 @@
         <v>101.8995879615612</v>
       </c>
       <c r="E76">
-        <v>101.1447121765166</v>
+        <v>101.1816261189208</v>
       </c>
       <c r="F76">
-        <v>102.5972685410186</v>
+        <v>102.6154907279845</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -1927,10 +1927,10 @@
         <v>102.1608600837188</v>
       </c>
       <c r="E77">
-        <v>101.4401986128229</v>
+        <v>101.4601150611088</v>
       </c>
       <c r="F77">
-        <v>102.8445806049583</v>
+        <v>102.8996740542081</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -1947,10 +1947,10 @@
         <v>102.0478732511678</v>
       </c>
       <c r="E78">
-        <v>101.3148096133255</v>
+        <v>101.3239748346128</v>
       </c>
       <c r="F78">
-        <v>102.7163385447086</v>
+        <v>102.7597623906338</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -1967,10 +1967,10 @@
         <v>101.8953972443522</v>
       </c>
       <c r="E79">
-        <v>101.170708532703</v>
+        <v>101.1572429836971</v>
       </c>
       <c r="F79">
-        <v>102.5835811646582</v>
+        <v>102.5925577840883</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -1987,10 +1987,10 @@
         <v>101.8491590484345</v>
       </c>
       <c r="E80">
-        <v>101.1599173948699</v>
+        <v>101.1088135352729</v>
       </c>
       <c r="F80">
-        <v>102.5448526952305</v>
+        <v>102.5639575354247</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2007,10 +2007,10 @@
         <v>101.6235772860025</v>
       </c>
       <c r="E81">
-        <v>100.939240825288</v>
+        <v>100.9187617838585</v>
       </c>
       <c r="F81">
-        <v>102.2937329846441</v>
+        <v>102.3624954446492</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2027,10 +2027,10 @@
         <v>101.6363875373307</v>
       </c>
       <c r="E82">
-        <v>100.9307362181115</v>
+        <v>100.9173033567278</v>
       </c>
       <c r="F82">
-        <v>102.343705519973</v>
+        <v>102.3217763095976</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -2047,10 +2047,10 @@
         <v>102.3151019151971</v>
       </c>
       <c r="E83">
-        <v>101.6463877011795</v>
+        <v>101.6248877523032</v>
       </c>
       <c r="F83">
-        <v>103.0354786919097</v>
+        <v>103.0000174068354</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2067,10 +2067,10 @@
         <v>102.1237322792421</v>
       </c>
       <c r="E84">
-        <v>101.4363085979279</v>
+        <v>101.4213183054429</v>
       </c>
       <c r="F84">
-        <v>102.7604239058582</v>
+        <v>102.803136209573</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -2087,10 +2087,10 @@
         <v>102.7692579282935</v>
       </c>
       <c r="E85">
-        <v>102.1132978923072</v>
+        <v>102.0954922318005</v>
       </c>
       <c r="F85">
-        <v>103.4374590342959</v>
+        <v>103.5347956702163</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -2107,10 +2107,10 @@
         <v>102.3014694397327</v>
       </c>
       <c r="E86">
-        <v>101.5522632648815</v>
+        <v>101.574996006682</v>
       </c>
       <c r="F86">
-        <v>103.0265859654067</v>
+        <v>103.0488094772215</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -2127,10 +2127,10 @@
         <v>102.2745383237832</v>
       </c>
       <c r="E87">
-        <v>101.570106369479</v>
+        <v>101.582918022208</v>
       </c>
       <c r="F87">
-        <v>102.9797524803961</v>
+        <v>103.0042416809286</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2147,10 +2147,10 @@
         <v>102.7664439827677</v>
       </c>
       <c r="E88">
-        <v>102.0793047333723</v>
+        <v>102.0814667549149</v>
       </c>
       <c r="F88">
-        <v>103.5054959173189</v>
+        <v>103.4930519433784</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2167,10 +2167,10 @@
         <v>103.6846178319243</v>
       </c>
       <c r="E89">
-        <v>102.9181206056183</v>
+        <v>103.0133946935776</v>
       </c>
       <c r="F89">
-        <v>104.3500023338057</v>
+        <v>104.3265286666334</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -2187,10 +2187,10 @@
         <v>103.6331510382959</v>
       </c>
       <c r="E90">
-        <v>102.9277819841413</v>
+        <v>102.9025387252115</v>
       </c>
       <c r="F90">
-        <v>104.3325318401918</v>
+        <v>104.3184171563082</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -2207,10 +2207,10 @@
         <v>104.3177890277553</v>
       </c>
       <c r="E91">
-        <v>103.5775256809891</v>
+        <v>103.6311158542124</v>
       </c>
       <c r="F91">
-        <v>105.0486618525938</v>
+        <v>105.0362982817167</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -2227,10 +2227,10 @@
         <v>105.0419173224172</v>
       </c>
       <c r="E92">
-        <v>104.3065611542166</v>
+        <v>104.3099252824664</v>
       </c>
       <c r="F92">
-        <v>105.7466769333659</v>
+        <v>105.7658090268649</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -2247,10 +2247,10 @@
         <v>104.9944924828975</v>
       </c>
       <c r="E93">
-        <v>104.3103127598464</v>
+        <v>104.3002698467505</v>
       </c>
       <c r="F93">
-        <v>105.6736750084613</v>
+        <v>105.6509609982366</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -2267,10 +2267,10 @@
         <v>105.2714962129347</v>
       </c>
       <c r="E94">
-        <v>104.6335701616995</v>
+        <v>104.5675664185025</v>
       </c>
       <c r="F94">
-        <v>105.9963120241285</v>
+        <v>105.9517621730631</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -2287,10 +2287,10 @@
         <v>106.0272991559107</v>
       </c>
       <c r="E95">
-        <v>105.3086912898524</v>
+        <v>105.3074807957714</v>
       </c>
       <c r="F95">
-        <v>106.6830730811679</v>
+        <v>106.7453218506773</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -2307,10 +2307,10 @@
         <v>106.555233731514</v>
       </c>
       <c r="E96">
-        <v>105.8910705728811</v>
+        <v>105.8249481866863</v>
       </c>
       <c r="F96">
-        <v>107.2521457153791</v>
+        <v>107.1884234304039</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -2327,10 +2327,10 @@
         <v>107.1219377798666</v>
       </c>
       <c r="E97">
-        <v>106.459100483577</v>
+        <v>106.4170827220652</v>
       </c>
       <c r="F97">
-        <v>107.8304067589977</v>
+        <v>107.7688751605456</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -2347,10 +2347,10 @@
         <v>106.8871573567382</v>
       </c>
       <c r="E98">
-        <v>106.2077025634197</v>
+        <v>106.1933491244294</v>
       </c>
       <c r="F98">
-        <v>107.6147051932386</v>
+        <v>107.5859124316488</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -2367,10 +2367,10 @@
         <v>107.2114826499776</v>
       </c>
       <c r="E99">
-        <v>106.5071309727215</v>
+        <v>106.4789321528627</v>
       </c>
       <c r="F99">
-        <v>107.9460132974194</v>
+        <v>107.9551844817337</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -2387,10 +2387,10 @@
         <v>107.5762883995121</v>
       </c>
       <c r="E100">
-        <v>106.8434672211346</v>
+        <v>106.886037529239</v>
       </c>
       <c r="F100">
-        <v>108.2295837012832</v>
+        <v>108.2984773185251</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -2407,10 +2407,10 @@
         <v>107.6122954328949</v>
       </c>
       <c r="E101">
-        <v>106.8783400168468</v>
+        <v>106.9289044011588</v>
       </c>
       <c r="F101">
-        <v>108.3268290660903</v>
+        <v>108.2809770904076</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -2427,10 +2427,10 @@
         <v>107.5188587905234</v>
       </c>
       <c r="E102">
-        <v>106.805705489604</v>
+        <v>106.8346365061483</v>
       </c>
       <c r="F102">
-        <v>108.2578915178192</v>
+        <v>108.3059765442484</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -2447,10 +2447,10 @@
         <v>107.6728991076946</v>
       </c>
       <c r="E103">
-        <v>106.9919632338275</v>
+        <v>106.9467864624686</v>
       </c>
       <c r="F103">
-        <v>108.393724980945</v>
+        <v>108.3870951172359</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -2467,10 +2467,10 @@
         <v>108.104958357304</v>
       </c>
       <c r="E104">
-        <v>107.4171041066081</v>
+        <v>107.4057924809653</v>
       </c>
       <c r="F104">
-        <v>108.8353350377148</v>
+        <v>108.8235986275153</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -2487,10 +2487,10 @@
         <v>108.2017083135553</v>
       </c>
       <c r="E105">
-        <v>107.5630717411407</v>
+        <v>107.4801142373561</v>
       </c>
       <c r="F105">
-        <v>108.8916252867404</v>
+        <v>108.987819836027</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -2507,10 +2507,10 @@
         <v>108.5309272667882</v>
       </c>
       <c r="E106">
-        <v>107.8688138889522</v>
+        <v>107.8626037549366</v>
       </c>
       <c r="F106">
-        <v>109.2084467946931</v>
+        <v>109.1967344508806</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -2527,10 +2527,10 @@
         <v>108.1880725265816</v>
       </c>
       <c r="E107">
-        <v>107.4826949568138</v>
+        <v>107.5042093044153</v>
       </c>
       <c r="F107">
-        <v>108.9301803811454</v>
+        <v>108.8646072882603</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -2547,10 +2547,10 @@
         <v>108.766919062403</v>
       </c>
       <c r="E108">
-        <v>108.0522937288157</v>
+        <v>108.1046126112829</v>
       </c>
       <c r="F108">
-        <v>109.4982939557343</v>
+        <v>109.4342918870756</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -2567,10 +2567,10 @@
         <v>109.1034696822857</v>
       </c>
       <c r="E109">
-        <v>108.3859190160971</v>
+        <v>108.4418166573534</v>
       </c>
       <c r="F109">
-        <v>109.844239118617</v>
+        <v>109.8256249803319</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -2587,10 +2587,10 @@
         <v>108.6146147084751</v>
       </c>
       <c r="E110">
-        <v>107.8658143794981</v>
+        <v>107.8957039424216</v>
       </c>
       <c r="F110">
-        <v>109.3370143956779</v>
+        <v>109.3142472711347</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -2607,10 +2607,10 @@
         <v>108.8718715824796</v>
       </c>
       <c r="E111">
-        <v>108.1122215681474</v>
+        <v>108.2160684772663</v>
       </c>
       <c r="F111">
-        <v>109.5900282194388</v>
+        <v>109.5730899812379</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -2627,10 +2627,10 @@
         <v>109.2501790046248</v>
       </c>
       <c r="E112">
-        <v>108.5790757351449</v>
+        <v>108.514385089221</v>
       </c>
       <c r="F112">
-        <v>109.9767693583087</v>
+        <v>109.9251012632235</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -2647,10 +2647,10 @@
         <v>109.0946065949522</v>
       </c>
       <c r="E113">
-        <v>108.3778138960137</v>
+        <v>108.3892679124983</v>
       </c>
       <c r="F113">
-        <v>109.7689509946741</v>
+        <v>109.8130515952955</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -2667,10 +2667,10 @@
         <v>109.2102553677619</v>
       </c>
       <c r="E114">
-        <v>108.4948077287535</v>
+        <v>108.4996612479911</v>
       </c>
       <c r="F114">
-        <v>109.9449015267268</v>
+        <v>109.9299696458994</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -2687,10 +2687,10 @@
         <v>109.7455828198247</v>
       </c>
       <c r="E115">
-        <v>109.050694886483</v>
+        <v>108.9933528711375</v>
       </c>
       <c r="F115">
-        <v>110.4147489802821</v>
+        <v>110.4244661163808</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -2707,10 +2707,10 @@
         <v>109.6872003657527</v>
       </c>
       <c r="E116">
-        <v>108.9796624486792</v>
+        <v>108.9307736186108</v>
       </c>
       <c r="F116">
-        <v>110.3815597735493</v>
+        <v>110.3663210145663</v>
       </c>
     </row>
     <row r="117" spans="1:6">
@@ -2727,10 +2727,10 @@
         <v>110.2626325069358</v>
       </c>
       <c r="E117">
-        <v>109.6195403725468</v>
+        <v>109.5772070249993</v>
       </c>
       <c r="F117">
-        <v>111.0006070441363</v>
+        <v>110.9582563451087</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -2747,10 +2747,10 @@
         <v>110.1263145260697</v>
       </c>
       <c r="E118">
-        <v>109.4482580966732</v>
+        <v>109.426462239188</v>
       </c>
       <c r="F118">
-        <v>110.763582011861</v>
+        <v>110.8088129544793</v>
       </c>
     </row>
     <row r="119" spans="1:6">
@@ -2767,10 +2767,10 @@
         <v>109.8786669756402</v>
       </c>
       <c r="E119">
-        <v>109.2317703163682</v>
+        <v>109.2575082424941</v>
       </c>
       <c r="F119">
-        <v>110.6169888760736</v>
+        <v>110.5640123628057</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -2787,10 +2787,10 @@
         <v>110.2544122068744</v>
       </c>
       <c r="E120">
-        <v>109.5580650658305</v>
+        <v>109.5789934020005</v>
       </c>
       <c r="F120">
-        <v>110.9552066971811</v>
+        <v>110.9497174851794</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -2807,10 +2807,10 @@
         <v>110.3802242420797</v>
       </c>
       <c r="E121">
-        <v>109.6825971610029</v>
+        <v>109.70005429931</v>
       </c>
       <c r="F121">
-        <v>111.090527395726</v>
+        <v>111.0820738747316</v>
       </c>
     </row>
     <row r="122" spans="1:6">
@@ -2827,10 +2827,10 @@
         <v>110.3999067443418</v>
       </c>
       <c r="E122">
-        <v>109.7197399767551</v>
+        <v>109.6928221810399</v>
       </c>
       <c r="F122">
-        <v>111.0817376894651</v>
+        <v>111.1072018388143</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -2844,10 +2844,10 @@
         <v>111.3279300677196</v>
       </c>
       <c r="E123">
-        <v>110.6019465765201</v>
+        <v>110.6132552605859</v>
       </c>
       <c r="F123">
-        <v>112.0418225759735</v>
+        <v>112.0344210582943</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -2861,10 +2861,10 @@
         <v>111.5548372711512</v>
       </c>
       <c r="E124">
-        <v>110.8765658587355</v>
+        <v>110.8925779419677</v>
       </c>
       <c r="F124">
-        <v>112.2783207766092</v>
+        <v>112.2602182168506</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -2878,10 +2878,10 @@
         <v>110.7459079046332</v>
       </c>
       <c r="E125">
-        <v>109.9962343424272</v>
+        <v>110.0594427664294</v>
       </c>
       <c r="F125">
-        <v>111.4950173946675</v>
+        <v>111.4444644360985</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -2895,10 +2895,10 @@
         <v>111.0328904849513</v>
       </c>
       <c r="E126">
-        <v>110.2719001480418</v>
+        <v>110.2825198304705</v>
       </c>
       <c r="F126">
-        <v>111.7903297563486</v>
+        <v>111.7798011073361</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -2912,10 +2912,10 @@
         <v>111.1147227369815</v>
       </c>
       <c r="E127">
-        <v>110.3248711544056</v>
+        <v>110.3565244634427</v>
       </c>
       <c r="F127">
-        <v>111.9152794299338</v>
+        <v>111.9050418263864</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -2929,10 +2929,10 @@
         <v>111.4479696700109</v>
       </c>
       <c r="E128">
-        <v>110.6394661869638</v>
+        <v>110.650117803802</v>
       </c>
       <c r="F128">
-        <v>112.2726451992771</v>
+        <v>112.2835192275966</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -2946,10 +2946,10 @@
         <v>111.9190226081632</v>
       </c>
       <c r="E129">
-        <v>110.9948356725616</v>
+        <v>110.9647454864722</v>
       </c>
       <c r="F129">
-        <v>112.8056420817375</v>
+        <v>112.7564464015201</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -2963,10 +2963,10 @@
         <v>111.838983935599</v>
       </c>
       <c r="E130">
-        <v>110.9428892875249</v>
+        <v>110.9064809742099</v>
       </c>
       <c r="F130">
-        <v>112.7502291717285</v>
+        <v>112.7822529706948</v>
       </c>
     </row>
     <row r="131" spans="1:6">
@@ -2980,10 +2980,10 @@
         <v>111.617052131952</v>
       </c>
       <c r="E131">
-        <v>110.6414987797315</v>
+        <v>110.547784839353</v>
       </c>
       <c r="F131">
-        <v>112.6521035203966</v>
+        <v>112.6818004070879</v>
       </c>
     </row>
     <row r="132" spans="1:6">
@@ -2997,10 +2997,10 @@
         <v>112.37455272019</v>
       </c>
       <c r="E132">
-        <v>111.3496300899289</v>
+        <v>111.2123716972143</v>
       </c>
       <c r="F132">
-        <v>113.5627301873892</v>
+        <v>113.4208191651074</v>
       </c>
     </row>
     <row r="133" spans="1:6">
@@ -3014,10 +3014,10 @@
         <v>111.7790363004907</v>
       </c>
       <c r="E133">
-        <v>110.7300999207734</v>
+        <v>110.4611109217767</v>
       </c>
       <c r="F133">
-        <v>113.1144752286714</v>
+        <v>112.9841057001046</v>
       </c>
     </row>
     <row r="134" spans="1:6">
@@ -3031,10 +3031,10 @@
         <v>112.322790524022</v>
       </c>
       <c r="E134">
-        <v>111.0827241585224</v>
+        <v>110.9380635380539</v>
       </c>
       <c r="F134">
-        <v>113.6934596816023</v>
+        <v>113.6557449409422</v>
       </c>
     </row>
   </sheetData>

</xml_diff>